<commit_message>
changes made on 23/09
</commit_message>
<xml_diff>
--- a/dashboard/Data/1_List of fuels.xlsx
+++ b/dashboard/Data/1_List of fuels.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>OSEMOSYS</t>
   </si>
@@ -208,6 +208,30 @@
   </si>
   <si>
     <t>Wind energy</t>
+  </si>
+  <si>
+    <t>Biomass for industry</t>
+  </si>
+  <si>
+    <t>Biomass for other sectors</t>
+  </si>
+  <si>
+    <t>Coal for industry</t>
+  </si>
+  <si>
+    <t>Coal for other sectors</t>
+  </si>
+  <si>
+    <t>BIO_IND</t>
+  </si>
+  <si>
+    <t>COA_IND</t>
+  </si>
+  <si>
+    <t>BIO_OTH</t>
+  </si>
+  <si>
+    <t>COA_OTH</t>
   </si>
 </sst>
 </file>
@@ -565,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,241 +628,273 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified lists of technologies
</commit_message>
<xml_diff>
--- a/dashboard/Data/1_List of fuels.xlsx
+++ b/dashboard/Data/1_List of fuels.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>OSEMOSYS</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Coal</t>
   </si>
   <si>
-    <t>Natural Gas</t>
-  </si>
-  <si>
     <t>Biomass</t>
   </si>
   <si>
@@ -42,9 +39,6 @@
     <t>Commercial electricity</t>
   </si>
   <si>
-    <t>Other oil products</t>
-  </si>
-  <si>
     <t>Gasoline</t>
   </si>
   <si>
@@ -81,21 +75,12 @@
     <t>HYD</t>
   </si>
   <si>
-    <t>IND_EN</t>
-  </si>
-  <si>
     <t>KER</t>
   </si>
   <si>
-    <t>NGS</t>
-  </si>
-  <si>
     <t>OIL</t>
   </si>
   <si>
-    <t>OILPROD</t>
-  </si>
-  <si>
     <t>OTH_EN</t>
   </si>
   <si>
@@ -117,24 +102,6 @@
     <t>SOL</t>
   </si>
   <si>
-    <t>TRA_AN_FREIGHT</t>
-  </si>
-  <si>
-    <t>TRA_AN_PSNG</t>
-  </si>
-  <si>
-    <t>TRA_RLW_FREIGHT</t>
-  </si>
-  <si>
-    <t>TRA_RLW_PSNG</t>
-  </si>
-  <si>
-    <t>TRA_ROAD_FREIGHT</t>
-  </si>
-  <si>
-    <t>TRA_ROAD_PSNG</t>
-  </si>
-  <si>
     <t>WND</t>
   </si>
   <si>
@@ -144,9 +111,6 @@
     <t>Commercial other energy</t>
   </si>
   <si>
-    <t>diesel</t>
-  </si>
-  <si>
     <t>Electricity for transmission</t>
   </si>
   <si>
@@ -162,9 +126,6 @@
     <t>Hydro</t>
   </si>
   <si>
-    <t>Industrial energy uses</t>
-  </si>
-  <si>
     <t>Oil</t>
   </si>
   <si>
@@ -189,49 +150,106 @@
     <t>Solar energy</t>
   </si>
   <si>
-    <t>Transportation freight aviation &amp; navigation - in Mton-km</t>
-  </si>
-  <si>
-    <t>Transportation passenger aviation &amp; navigation - in Mpassenger-km</t>
-  </si>
-  <si>
-    <t>Transportation railway freight - in Mton-km</t>
-  </si>
-  <si>
-    <t>Transportation passenger railway - in Mpassenger - km</t>
-  </si>
-  <si>
-    <t>Transportation road freight - in Mton-km</t>
-  </si>
-  <si>
-    <t>Transportation road passenger - in Mpassenger-km</t>
-  </si>
-  <si>
     <t>Wind energy</t>
   </si>
   <si>
-    <t>Biomass for industry</t>
-  </si>
-  <si>
-    <t>Biomass for other sectors</t>
-  </si>
-  <si>
-    <t>Coal for industry</t>
-  </si>
-  <si>
-    <t>Coal for other sectors</t>
-  </si>
-  <si>
-    <t>BIO_IND</t>
-  </si>
-  <si>
-    <t>COA_IND</t>
-  </si>
-  <si>
-    <t>BIO_OTH</t>
-  </si>
-  <si>
-    <t>COA_OTH</t>
+    <t>BIODSL</t>
+  </si>
+  <si>
+    <t>BIOGSL</t>
+  </si>
+  <si>
+    <t>Biodiesel</t>
+  </si>
+  <si>
+    <t>Bioethanol</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Industry cement and non-metal</t>
+  </si>
+  <si>
+    <t>IND_CHEM</t>
+  </si>
+  <si>
+    <t>IND_CMNT</t>
+  </si>
+  <si>
+    <t>IND_FOOD</t>
+  </si>
+  <si>
+    <t>IND_OTH</t>
+  </si>
+  <si>
+    <t>IND_TEXT</t>
+  </si>
+  <si>
+    <t>Industry food</t>
+  </si>
+  <si>
+    <t>Industry chemical and fertilizers</t>
+  </si>
+  <si>
+    <t>Industry other</t>
+  </si>
+  <si>
+    <t>Industry textile</t>
+  </si>
+  <si>
+    <t>NGS_001</t>
+  </si>
+  <si>
+    <t>NGS_002</t>
+  </si>
+  <si>
+    <t>Natural Gas for distribution</t>
+  </si>
+  <si>
+    <t>Natural Gas final</t>
+  </si>
+  <si>
+    <t>RE_FUEL</t>
+  </si>
+  <si>
+    <t>Dummy renewable fuel</t>
+  </si>
+  <si>
+    <t>TRA_AIR_FREIGHT</t>
+  </si>
+  <si>
+    <t>TRA_AIR_PSNG</t>
+  </si>
+  <si>
+    <t>Transportation aviation freight - in Mton-km</t>
+  </si>
+  <si>
+    <t>Transportation aviation passenger - in Mpassenger-km</t>
+  </si>
+  <si>
+    <t>Transportation land freight - in Mton-km</t>
+  </si>
+  <si>
+    <t>TRA_LAND_FREIGHT</t>
+  </si>
+  <si>
+    <t>TRA_LAND_PSNG</t>
+  </si>
+  <si>
+    <t>TRA_SHIP_FREIGHT</t>
+  </si>
+  <si>
+    <t>TRA_SHIP_PSNG</t>
+  </si>
+  <si>
+    <t>Transportation ship passenger - in thousands passengers</t>
+  </si>
+  <si>
+    <t>Transportation ship freight - in thousands tonnes</t>
+  </si>
+  <si>
+    <t>Transportation land passenger - in Mpassenger - km</t>
   </si>
 </sst>
 </file>
@@ -589,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -606,7 +624,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -620,26 +638,26 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -647,28 +665,28 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -676,7 +694,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -684,7 +702,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -692,7 +710,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -700,7 +718,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -708,7 +726,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -716,7 +734,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
@@ -724,178 +742,202 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated lists of techs and RES
</commit_message>
<xml_diff>
--- a/dashboard/Data/1_List of fuels.xlsx
+++ b/dashboard/Data/1_List of fuels.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>OSEMOSYS</t>
   </si>
@@ -250,6 +250,42 @@
   </si>
   <si>
     <t>Transportation land passenger - in Mpassenger - km</t>
+  </si>
+  <si>
+    <t>All transportation by bus</t>
+  </si>
+  <si>
+    <t>TRA_BUS</t>
+  </si>
+  <si>
+    <t>All transportation by car</t>
+  </si>
+  <si>
+    <t>TRA_CAR</t>
+  </si>
+  <si>
+    <t>All transportation by motorcycle</t>
+  </si>
+  <si>
+    <t>TRA_MCY</t>
+  </si>
+  <si>
+    <t>All railway passenger transportation</t>
+  </si>
+  <si>
+    <t>All railway freight transportation</t>
+  </si>
+  <si>
+    <t>TRA_TRAIN_PSNG</t>
+  </si>
+  <si>
+    <t>TRA_TRAIN_FREIGHT</t>
+  </si>
+  <si>
+    <t>All truck transportation</t>
+  </si>
+  <si>
+    <t>TRA_TRUCK</t>
   </si>
 </sst>
 </file>
@@ -607,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -934,9 +970,57 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>